<commit_message>
"Korea, South" sanitized to "Korea South" in py and csv's
</commit_message>
<xml_diff>
--- a/population_and_lockdown_table.xlsx
+++ b/population_and_lockdown_table.xlsx
@@ -439,6 +439,9 @@
     <t xml:space="preserve">Kenya</t>
   </si>
   <si>
+    <t xml:space="preserve">South Korea</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kosovo</t>
   </si>
   <si>
@@ -671,9 +674,6 @@
   </si>
   <si>
     <t xml:space="preserve">South Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Korea</t>
   </si>
   <si>
     <t xml:space="preserve">South Sudan</t>
@@ -806,6 +806,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -893,13 +894,13 @@
   </sheetPr>
   <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A156" activeCellId="0" sqref="A156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.19"/>
@@ -1858,13 +1859,7 @@
         <v>139</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>1845000</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>19</v>
+        <v>51269185</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,21 +1867,27 @@
         <v>140</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>4270571</v>
+        <v>1845000</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <v>4270571</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B93" s="0" t="n">
-        <v>6524195</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +1895,7 @@
         <v>143</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>7275560</v>
+        <v>6524195</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,7 +1903,7 @@
         <v>144</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>1886198</v>
+        <v>7275560</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,21 +1911,21 @@
         <v>145</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>6825445</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>34</v>
+        <v>1886198</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>6825445</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B97" s="0" t="n">
-        <v>2142249</v>
+      <c r="D97" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1932,13 +1933,7 @@
         <v>148</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>5057681</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>126</v>
+        <v>2142249</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,13 +1941,13 @@
         <v>149</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>6871292</v>
+        <v>5057681</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>43</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1960,7 +1955,13 @@
         <v>150</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>38128</v>
+        <v>6871292</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,21 +1969,21 @@
         <v>151</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>2722289</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>152</v>
+        <v>38128</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>2722289</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B102" s="0" t="n">
-        <v>625978</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,13 +1991,7 @@
         <v>154</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>27691018</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>80</v>
+        <v>625978</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,7 +1999,13 @@
         <v>155</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>19129952</v>
+        <v>27691018</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,21 +2013,21 @@
         <v>156</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>32365999</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>157</v>
+        <v>19129952</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>32365999</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="B106" s="0" t="n">
-        <v>540544</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,7 +2035,7 @@
         <v>159</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>20250833</v>
+        <v>540544</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,7 +2043,7 @@
         <v>160</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>441543</v>
+        <v>20250833</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,7 +2051,7 @@
         <v>161</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>4649658</v>
+        <v>441543</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2058,7 +2059,7 @@
         <v>162</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>1271768</v>
+        <v>4649658</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,13 +2067,7 @@
         <v>163</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>128932753</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>7</v>
+        <v>1271768</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,7 +2075,13 @@
         <v>164</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>4033963</v>
+        <v>128932753</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,7 +2089,7 @@
         <v>165</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>39242</v>
+        <v>4033963</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2096,27 +2097,21 @@
         <v>166</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>3278290</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>23</v>
+        <v>39242</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>3278290</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B115" s="0" t="n">
-        <v>628066</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D115" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,21 +2119,27 @@
         <v>169</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>36910560</v>
+        <v>628066</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>170</v>
+        <v>43</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>36910560</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="B117" s="0" t="n">
-        <v>31255435</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2146,35 +2147,35 @@
         <v>172</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>2540905</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>19</v>
+        <v>31255435</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>2540905</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B119" s="0" t="n">
-        <v>29136808</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D119" s="1" t="s">
-        <v>175</v>
+        <v>19</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>29136808</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="B120" s="0" t="n">
-        <v>17134872</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2182,13 +2183,7 @@
         <v>177</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>4822233</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>10</v>
+        <v>17134872</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2191,13 @@
         <v>178</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>6624554</v>
+        <v>4822233</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,7 +2205,7 @@
         <v>179</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>24206644</v>
+        <v>6624554</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,13 +2213,7 @@
         <v>180</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>206139589</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>107</v>
+        <v>24206644</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2226,7 +2221,13 @@
         <v>181</v>
       </c>
       <c r="B125" s="0" t="n">
-        <v>2083374</v>
+        <v>206139589</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,7 +2235,7 @@
         <v>182</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>5421241</v>
+        <v>2083374</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,41 +2243,35 @@
         <v>183</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>5106626</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>184</v>
+        <v>5421241</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>5106626</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B128" s="0" t="n">
-        <v>220892340</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>220892340</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B129" s="0" t="n">
-        <v>4314767</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,7 +2279,13 @@
         <v>188</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>8947024</v>
+        <v>4314767</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,13 +2293,7 @@
         <v>189</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>7132538</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>35</v>
+        <v>8947024</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,13 +2301,13 @@
         <v>190</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>32971854</v>
+        <v>7132538</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,27 +2315,27 @@
         <v>191</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>109581078</v>
+        <v>32971854</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>173</v>
+        <v>23</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>192</v>
+        <v>70</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B134" s="0" t="n">
+        <v>109581078</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B134" s="0" t="n">
-        <v>37846611</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2348,13 +2343,13 @@
         <v>194</v>
       </c>
       <c r="B135" s="0" t="n">
-        <v>10196709</v>
+        <v>37846611</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,41 +2357,41 @@
         <v>195</v>
       </c>
       <c r="B136" s="0" t="n">
-        <v>2881053</v>
+        <v>10196709</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>196</v>
+        <v>15</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B137" s="0" t="n">
+        <v>2881053</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B137" s="0" t="n">
-        <v>19237691</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="D137" s="1" t="s">
-        <v>198</v>
+        <v>43</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B138" s="0" t="n">
+        <v>19237691</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="B138" s="0" t="n">
-        <v>145934462</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,21 +2399,27 @@
         <v>200</v>
       </c>
       <c r="B139" s="0" t="n">
-        <v>12952218</v>
+        <v>145934462</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>201</v>
+        <v>106</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>75</v>
+        <v>199</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B140" s="0" t="n">
+        <v>12952218</v>
+      </c>
+      <c r="C140" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B140" s="0" t="n">
-        <v>53199</v>
+      <c r="D140" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2426,7 +2427,7 @@
         <v>203</v>
       </c>
       <c r="B141" s="0" t="n">
-        <v>183627</v>
+        <v>53199</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,7 +2435,7 @@
         <v>204</v>
       </c>
       <c r="B142" s="0" t="n">
-        <v>110940</v>
+        <v>183627</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2442,7 +2443,7 @@
         <v>205</v>
       </c>
       <c r="B143" s="0" t="n">
-        <v>33931</v>
+        <v>110940</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2450,7 +2451,7 @@
         <v>206</v>
       </c>
       <c r="B144" s="0" t="n">
-        <v>219159</v>
+        <v>33931</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2458,7 +2459,7 @@
         <v>207</v>
       </c>
       <c r="B145" s="0" t="n">
-        <v>34813871</v>
+        <v>219159</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,7 +2467,7 @@
         <v>208</v>
       </c>
       <c r="B146" s="0" t="n">
-        <v>16743927</v>
+        <v>34813871</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,13 +2475,7 @@
         <v>209</v>
       </c>
       <c r="B147" s="0" t="n">
-        <v>8737371</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>103</v>
+        <v>16743927</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,7 +2483,13 @@
         <v>210</v>
       </c>
       <c r="B148" s="0" t="n">
-        <v>98347</v>
+        <v>8737371</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,7 +2497,7 @@
         <v>211</v>
       </c>
       <c r="B149" s="0" t="n">
-        <v>7976983</v>
+        <v>98347</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2504,13 +2505,7 @@
         <v>212</v>
       </c>
       <c r="B150" s="0" t="n">
-        <v>5850342</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>7</v>
+        <v>7976983</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,7 +2513,13 @@
         <v>213</v>
       </c>
       <c r="B151" s="0" t="n">
-        <v>5459642</v>
+        <v>5850342</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,7 +2527,7 @@
         <v>214</v>
       </c>
       <c r="B152" s="0" t="n">
-        <v>2078938</v>
+        <v>5459642</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2534,7 +2535,7 @@
         <v>215</v>
       </c>
       <c r="B153" s="0" t="n">
-        <v>15893222</v>
+        <v>2078938</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2542,13 +2543,7 @@
         <v>216</v>
       </c>
       <c r="B154" s="0" t="n">
-        <v>59308690</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>50</v>
+        <v>15893222</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2556,7 +2551,13 @@
         <v>217</v>
       </c>
       <c r="B155" s="0" t="n">
-        <v>51269185</v>
+        <v>59308690</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2578,7 +2579,7 @@
         <v>124</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>